<commit_message>
add apiCategories excel file to show the categories that can be searched
</commit_message>
<xml_diff>
--- a/apiCategories.xlsx
+++ b/apiCategories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Semester11\FrontendDev\DafunnyButton\DaFunnyButton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{425A3E07-51B2-445D-968C-232614FDF12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C923D-F177-4B1F-9416-6D125598B17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0AB5CB25-1172-4B12-9293-F653B9919642}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0AB5CB25-1172-4B12-9293-F653B9919642}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -488,7 +499,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +630,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:D13">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>